<commit_message>
Went through and did first runs across almost all the budget documents. Also divided the scheduling file across each of the platforms.
</commit_message>
<xml_diff>
--- a/FOIA SAR data/LW155 M777/All Docs_M777 Data Draw.xlsx
+++ b/FOIA SAR data/LW155 M777/All Docs_M777 Data Draw.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\2015-09 Joint Development\Research\XM777\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Greg Sanders\Documents\Development\R-scripts-and-data\FOIA SAR data\LW155 M777\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="10560" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="10560" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="All Years_vol2.summary" sheetId="1" r:id="rId1"/>
-    <sheet name="1999_PMC_BOOK.summary " sheetId="2" r:id="rId2"/>
+    <sheet name="1999_PMC_BOOK.summary" sheetId="2" r:id="rId2"/>
     <sheet name="All Years_RDTEN_BA_4" sheetId="4" r:id="rId3"/>
     <sheet name="All Years_wtcv" sheetId="5" r:id="rId4"/>
-    <sheet name="Marine Corps Data" sheetId="7" r:id="rId5"/>
+    <sheet name="All Years_N_BA4" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -2851,207 +2851,213 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="C4" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="11">
         <v>35827</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
+      <c r="E5">
+        <v>70</v>
+      </c>
+      <c r="F5">
+        <v>120</v>
+      </c>
       <c r="G5">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="H5">
         <v>120</v>
       </c>
       <c r="I5">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="J5">
-        <v>120</v>
-      </c>
-      <c r="K5">
-        <v>96</v>
-      </c>
-      <c r="L5">
         <v>526</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>86.3</v>
+      </c>
       <c r="F6">
-        <v>10</v>
+        <v>116.8</v>
       </c>
       <c r="G6">
-        <v>86.3</v>
+        <v>121.6</v>
       </c>
       <c r="H6">
-        <v>116.8</v>
+        <v>117.7</v>
       </c>
       <c r="I6">
-        <v>121.6</v>
+        <v>100</v>
       </c>
       <c r="J6">
-        <v>117.7</v>
-      </c>
-      <c r="K6">
-        <v>100</v>
-      </c>
-      <c r="L6">
         <v>552.4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>86.3</v>
+      </c>
       <c r="F9">
-        <v>10</v>
+        <v>116.8</v>
       </c>
       <c r="G9">
-        <v>86.3</v>
+        <v>121.6</v>
       </c>
       <c r="H9">
-        <v>116.8</v>
+        <v>117.7</v>
       </c>
       <c r="I9">
-        <v>121.6</v>
+        <v>100</v>
       </c>
       <c r="J9">
-        <v>117.7</v>
-      </c>
-      <c r="K9">
-        <v>100</v>
-      </c>
-      <c r="L9">
         <v>552.4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
+      <c r="F10">
+        <v>3.4</v>
+      </c>
+      <c r="G10">
+        <v>5.9</v>
+      </c>
       <c r="H10">
-        <v>3.4</v>
+        <v>5</v>
       </c>
       <c r="I10">
-        <v>5.9</v>
+        <v>2.6</v>
       </c>
       <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="K10">
-        <v>2.6</v>
-      </c>
-      <c r="L10">
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>86.3</v>
+      </c>
       <c r="F11">
-        <v>10</v>
+        <v>120.2</v>
       </c>
       <c r="G11">
-        <v>86.3</v>
+        <v>127.5</v>
       </c>
       <c r="H11">
-        <v>120.2</v>
+        <v>122.7</v>
       </c>
       <c r="I11">
-        <v>127.5</v>
+        <v>102.6</v>
       </c>
       <c r="J11">
-        <v>122.7</v>
-      </c>
-      <c r="K11">
-        <v>102.6</v>
-      </c>
-      <c r="L11">
         <v>569.29999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="L12">
+      <c r="J12">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
+      <c r="E13">
+        <v>1.2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
       <c r="G13">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -3060,12 +3066,6 @@
         <v>1</v>
       </c>
       <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -3077,10 +3077,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3112,460 +3112,460 @@
         <v>36</v>
       </c>
     </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>29</v>
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4">
+        <v>32332</v>
+      </c>
+      <c r="C4" s="4">
+        <v>23237</v>
+      </c>
+      <c r="D4" s="4">
+        <v>12105</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B5" s="4">
-        <v>32332</v>
+        <v>569</v>
       </c>
       <c r="C5" s="4">
-        <v>23237</v>
+        <v>3880</v>
       </c>
       <c r="D5" s="4">
-        <v>12105</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="4">
+        <v>31763</v>
+      </c>
+      <c r="C6" s="4">
+        <v>27117</v>
+      </c>
+      <c r="D6" s="4">
+        <v>13119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>11105</v>
+      </c>
+      <c r="F9">
+        <v>90055</v>
+      </c>
+      <c r="G9">
+        <v>197065</v>
+      </c>
+      <c r="H9">
+        <v>142352</v>
+      </c>
+      <c r="I9">
+        <v>238</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>440815</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="4">
+        <v>27.117000000000001</v>
+      </c>
+      <c r="C14" s="4">
+        <v>13.119</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="4">
-        <v>569</v>
-      </c>
-      <c r="C6" s="4">
-        <v>3880</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="4">
-        <v>31763</v>
-      </c>
-      <c r="C7" s="4">
-        <v>27117</v>
-      </c>
-      <c r="D7" s="4">
-        <v>13119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>11105</v>
-      </c>
-      <c r="F10">
-        <v>90055</v>
-      </c>
-      <c r="G10">
-        <v>197065</v>
-      </c>
-      <c r="H10">
-        <v>142352</v>
-      </c>
-      <c r="I10">
-        <v>238</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>440815</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B16" s="4">
-        <v>27.117000000000001</v>
-      </c>
-      <c r="C16" s="4">
-        <v>13.119</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="4"/>
+        <v>60</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B18" s="4">
-        <v>0.52700000000000002</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+        <v>9.4E-2</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.121</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.29699999999999999</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.151</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="D19" s="4">
+        <v>18.5</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B20" s="4">
-        <v>9.4E-2</v>
+        <v>26.344999999999999</v>
       </c>
       <c r="C20" s="4">
-        <v>0.121</v>
+        <v>12.997999999999999</v>
       </c>
       <c r="D20" s="4">
-        <v>0.29699999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="4">
-        <v>0.151</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4">
-        <v>18.5</v>
+        <v>18.202999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="4">
-        <v>26.344999999999999</v>
-      </c>
-      <c r="C22" s="4">
-        <v>12.997999999999999</v>
-      </c>
-      <c r="D22" s="4">
-        <v>18.202999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B22" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="H22" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="I24" s="9" t="s">
+      <c r="I22" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="J24" s="6" t="s">
+      <c r="J22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="6" t="s">
+      <c r="K22" s="6" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>11.004</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>46</v>
       </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
+      <c r="B27">
         <v>11.004</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>62.643000000000001</v>
+      </c>
+      <c r="E27">
+        <v>111.489</v>
+      </c>
+      <c r="F27">
+        <v>179.32499999999999</v>
+      </c>
+      <c r="G27">
+        <v>181.18299999999999</v>
+      </c>
+      <c r="H27">
+        <v>75.363</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>621.00699999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="B30" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="E30" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="F30" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="G30" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="H30" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J30" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J28" s="6" t="s">
+      <c r="K30" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>46</v>
       </c>
-      <c r="B29">
-        <v>11.004</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>62.643000000000001</v>
-      </c>
-      <c r="E29">
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>62.02</v>
+      </c>
+      <c r="D31">
         <v>111.489</v>
       </c>
-      <c r="F29">
-        <v>179.32499999999999</v>
-      </c>
-      <c r="G29">
-        <v>181.18299999999999</v>
-      </c>
-      <c r="H29">
-        <v>75.363</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>621.00699999999995</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>62.02</v>
-      </c>
-      <c r="D33">
-        <v>111.489</v>
-      </c>
-      <c r="E33">
+      <c r="E31">
         <v>175.54300000000001</v>
       </c>
-      <c r="F33">
+      <c r="F31">
         <v>177.071</v>
       </c>
-      <c r="G33">
+      <c r="G31">
         <v>73.584999999999994</v>
       </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
         <v>599.70799999999997</v>
       </c>
     </row>
@@ -6939,8 +6939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Processed another sheet, but solitary dates aren't joining properly.
</commit_message>
<xml_diff>
--- a/FOIA SAR data/LW155 M777/All Docs_M777 Data Draw.xlsx
+++ b/FOIA SAR data/LW155 M777/All Docs_M777 Data Draw.xlsx
@@ -783,10 +783,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3607,12 +3607,12 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -3857,12 +3857,12 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -4054,12 +4054,12 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
@@ -4275,12 +4275,12 @@
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
@@ -4553,12 +4553,12 @@
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="14" t="s">
+      <c r="A68" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
@@ -4771,12 +4771,12 @@
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="s">
+      <c r="A82" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B82" s="14"/>
-      <c r="C82" s="14"/>
-      <c r="D82" s="14"/>
+      <c r="B82" s="15"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="15"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
@@ -5290,12 +5290,12 @@
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A111" s="14" t="s">
+      <c r="A111" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B111" s="14"/>
-      <c r="C111" s="14"/>
-      <c r="D111" s="14"/>
+      <c r="B111" s="15"/>
+      <c r="C111" s="15"/>
+      <c r="D111" s="15"/>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
@@ -5553,12 +5553,12 @@
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A125" s="14" t="s">
+      <c r="A125" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B125" s="14"/>
-      <c r="C125" s="14"/>
-      <c r="D125" s="14"/>
+      <c r="B125" s="15"/>
+      <c r="C125" s="15"/>
+      <c r="D125" s="15"/>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
@@ -5798,12 +5798,12 @@
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A139" s="14" t="s">
+      <c r="A139" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B139" s="14"/>
-      <c r="C139" s="14"/>
-      <c r="D139" s="14"/>
+      <c r="B139" s="15"/>
+      <c r="C139" s="15"/>
+      <c r="D139" s="15"/>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
@@ -5971,12 +5971,12 @@
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A153" s="14" t="s">
+      <c r="A153" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B153" s="14"/>
-      <c r="C153" s="14"/>
-      <c r="D153" s="14"/>
+      <c r="B153" s="15"/>
+      <c r="C153" s="15"/>
+      <c r="D153" s="15"/>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
@@ -6126,12 +6126,12 @@
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A167" s="14" t="s">
+      <c r="A167" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B167" s="14"/>
-      <c r="C167" s="14"/>
-      <c r="D167" s="14"/>
+      <c r="B167" s="15"/>
+      <c r="C167" s="15"/>
+      <c r="D167" s="15"/>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
@@ -6314,12 +6314,12 @@
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A181" s="15" t="s">
+      <c r="A181" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B181" s="15"/>
-      <c r="C181" s="15"/>
-      <c r="D181" s="15"/>
+      <c r="B181" s="14"/>
+      <c r="C181" s="14"/>
+      <c r="D181" s="14"/>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
@@ -6616,12 +6616,12 @@
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A192" s="15" t="s">
+      <c r="A192" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B192" s="15"/>
-      <c r="C192" s="15"/>
-      <c r="D192" s="15"/>
+      <c r="B192" s="14"/>
+      <c r="C192" s="14"/>
+      <c r="D192" s="14"/>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
@@ -6909,13 +6909,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A192:D192"/>
-    <mergeCell ref="A111:D111"/>
-    <mergeCell ref="A125:D125"/>
-    <mergeCell ref="A139:D139"/>
-    <mergeCell ref="A153:D153"/>
-    <mergeCell ref="A167:D167"/>
-    <mergeCell ref="A181:D181"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="B94:D94"/>
     <mergeCell ref="E94:G94"/>
     <mergeCell ref="H94:J94"/>
@@ -6924,11 +6922,13 @@
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A68:D68"/>
     <mergeCell ref="A82:D82"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A192:D192"/>
+    <mergeCell ref="A111:D111"/>
+    <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A139:D139"/>
+    <mergeCell ref="A153:D153"/>
+    <mergeCell ref="A167:D167"/>
+    <mergeCell ref="A181:D181"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6937,10 +6937,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7527,699 +7527,664 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>43</v>
-      </c>
-    </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>200</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H34" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="I34" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="J34" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="K34" s="12" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>200</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>201</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
         <v>11105</v>
       </c>
-      <c r="F35">
+      <c r="F36">
         <v>90055</v>
       </c>
-      <c r="G35">
+      <c r="G36">
         <v>197065</v>
       </c>
-      <c r="H35">
+      <c r="H36">
         <v>142352</v>
       </c>
-      <c r="I35">
+      <c r="I36">
         <v>238</v>
       </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
         <v>440815</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
         <v>37043</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>193</v>
-      </c>
-      <c r="B39" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E40" t="s">
-        <v>31</v>
-      </c>
-      <c r="F40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G40" t="s">
-        <v>198</v>
-      </c>
-      <c r="H40" t="s">
-        <v>199</v>
-      </c>
-      <c r="I40" t="s">
-        <v>65</v>
-      </c>
-      <c r="J40" t="s">
-        <v>12</v>
-      </c>
-      <c r="K40" t="s">
-        <v>85</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>197</v>
-      </c>
-      <c r="B41">
-        <v>26.344999999999999</v>
-      </c>
-      <c r="C41">
-        <v>12.997999999999999</v>
-      </c>
-      <c r="D41">
-        <v>18.202999999999999</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <v>57.545999999999999</v>
+        <v>196</v>
+      </c>
+      <c r="B41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" t="s">
+        <v>198</v>
+      </c>
+      <c r="H41" t="s">
+        <v>199</v>
+      </c>
+      <c r="I41" t="s">
+        <v>65</v>
+      </c>
+      <c r="J41" t="s">
+        <v>12</v>
+      </c>
+      <c r="K41" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>197</v>
+      </c>
+      <c r="B42">
+        <v>26.344999999999999</v>
+      </c>
+      <c r="C42">
+        <v>12.997999999999999</v>
+      </c>
+      <c r="D42">
+        <v>18.202999999999999</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>57.545999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>200</v>
-      </c>
-      <c r="B43" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" t="s">
-        <v>29</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" t="s">
-        <v>31</v>
-      </c>
-      <c r="F43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G43" t="s">
-        <v>198</v>
-      </c>
-      <c r="H43" t="s">
-        <v>199</v>
-      </c>
-      <c r="I43" t="s">
-        <v>65</v>
-      </c>
-      <c r="J43" t="s">
-        <v>12</v>
-      </c>
-      <c r="K43" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>200</v>
+      </c>
+      <c r="B44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G44" t="s">
+        <v>198</v>
+      </c>
+      <c r="H44" t="s">
+        <v>199</v>
+      </c>
+      <c r="I44" t="s">
+        <v>65</v>
+      </c>
+      <c r="J44" t="s">
+        <v>12</v>
+      </c>
+      <c r="K44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>201</v>
       </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="C44">
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
         <v>11.004</v>
       </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-      <c r="J44">
-        <v>0</v>
-      </c>
-      <c r="K44" t="s">
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
         <v>37288</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>193</v>
-      </c>
-      <c r="B48" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>196</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D49" t="s">
-        <v>31</v>
-      </c>
-      <c r="E49" t="s">
-        <v>32</v>
-      </c>
-      <c r="F49" t="s">
-        <v>198</v>
-      </c>
-      <c r="G49" t="s">
-        <v>199</v>
-      </c>
-      <c r="H49" t="s">
-        <v>65</v>
-      </c>
-      <c r="I49" t="s">
-        <v>12</v>
-      </c>
-      <c r="J49" t="s">
-        <v>85</v>
+        <v>193</v>
+      </c>
+      <c r="B49" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>197</v>
-      </c>
-      <c r="B50">
-        <v>13.446</v>
-      </c>
-      <c r="C50">
-        <v>13.085000000000001</v>
-      </c>
-      <c r="D50">
-        <v>11.632999999999999</v>
-      </c>
-      <c r="E50">
-        <v>5.97</v>
-      </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-      <c r="I50">
-        <v>0</v>
-      </c>
-      <c r="J50">
-        <v>44.134</v>
+        <v>196</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F50" t="s">
+        <v>198</v>
+      </c>
+      <c r="G50" t="s">
+        <v>199</v>
+      </c>
+      <c r="H50" t="s">
+        <v>65</v>
+      </c>
+      <c r="I50" t="s">
+        <v>12</v>
+      </c>
+      <c r="J50" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>197</v>
+      </c>
+      <c r="B51">
+        <v>13.446</v>
+      </c>
+      <c r="C51">
+        <v>13.085000000000001</v>
+      </c>
+      <c r="D51">
+        <v>11.632999999999999</v>
+      </c>
+      <c r="E51">
+        <v>5.97</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>44.134</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>200</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D52" t="s">
-        <v>31</v>
-      </c>
-      <c r="E52" t="s">
-        <v>32</v>
-      </c>
-      <c r="F52" t="s">
-        <v>198</v>
-      </c>
-      <c r="G52" t="s">
-        <v>199</v>
-      </c>
-      <c r="H52" t="s">
-        <v>65</v>
-      </c>
-      <c r="I52" t="s">
-        <v>12</v>
-      </c>
-      <c r="J52" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>200</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" t="s">
+        <v>31</v>
+      </c>
+      <c r="E53" t="s">
+        <v>32</v>
+      </c>
+      <c r="F53" t="s">
+        <v>198</v>
+      </c>
+      <c r="G53" t="s">
+        <v>199</v>
+      </c>
+      <c r="H53" t="s">
+        <v>65</v>
+      </c>
+      <c r="I53" t="s">
+        <v>12</v>
+      </c>
+      <c r="J53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>201</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <v>11.004</v>
       </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
-      <c r="D53">
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
         <v>62.643000000000001</v>
       </c>
-      <c r="E53">
+      <c r="E54">
         <v>111.489</v>
       </c>
-      <c r="F53">
+      <c r="F54">
         <v>179.32499999999999</v>
       </c>
-      <c r="G53">
+      <c r="G54">
         <v>181.18299999999999</v>
       </c>
-      <c r="H53">
+      <c r="H54">
         <v>75.363</v>
       </c>
-      <c r="I53">
-        <v>0</v>
-      </c>
-      <c r="J53">
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
         <v>621.00699999999995</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="11">
         <v>37653</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>193</v>
-      </c>
-      <c r="B58" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>196</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C59" t="s">
-        <v>31</v>
-      </c>
-      <c r="D59" t="s">
-        <v>32</v>
-      </c>
-      <c r="E59" t="s">
-        <v>198</v>
-      </c>
-      <c r="F59" t="s">
-        <v>199</v>
-      </c>
-      <c r="G59" t="s">
-        <v>65</v>
-      </c>
-      <c r="H59" t="s">
-        <v>104</v>
-      </c>
-      <c r="I59" t="s">
-        <v>105</v>
-      </c>
-      <c r="J59" t="s">
-        <v>12</v>
-      </c>
-      <c r="K59" t="s">
-        <v>85</v>
+        <v>193</v>
+      </c>
+      <c r="B59" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>197</v>
-      </c>
-      <c r="B60">
-        <v>14.558</v>
-      </c>
-      <c r="C60">
-        <v>11.367000000000001</v>
-      </c>
-      <c r="D60">
-        <v>5.8280000000000003</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
-      <c r="G60">
-        <v>0</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
-      <c r="K60">
-        <v>31.753</v>
+        <v>196</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60" t="s">
+        <v>31</v>
+      </c>
+      <c r="D60" t="s">
+        <v>32</v>
+      </c>
+      <c r="E60" t="s">
+        <v>198</v>
+      </c>
+      <c r="F60" t="s">
+        <v>199</v>
+      </c>
+      <c r="G60" t="s">
+        <v>65</v>
+      </c>
+      <c r="H60" t="s">
+        <v>104</v>
+      </c>
+      <c r="I60" t="s">
+        <v>105</v>
+      </c>
+      <c r="J60" t="s">
+        <v>12</v>
+      </c>
+      <c r="K60" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>197</v>
+      </c>
+      <c r="B61">
+        <v>14.558</v>
+      </c>
+      <c r="C61">
+        <v>11.367000000000001</v>
+      </c>
+      <c r="D61">
+        <v>5.8280000000000003</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>31.753</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>200</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C62" t="s">
-        <v>31</v>
-      </c>
-      <c r="D62" t="s">
-        <v>32</v>
-      </c>
-      <c r="E62" t="s">
-        <v>198</v>
-      </c>
-      <c r="F62" t="s">
-        <v>199</v>
-      </c>
-      <c r="G62" t="s">
-        <v>65</v>
-      </c>
-      <c r="H62" t="s">
-        <v>104</v>
-      </c>
-      <c r="I62" t="s">
-        <v>105</v>
-      </c>
-      <c r="J62" t="s">
-        <v>12</v>
-      </c>
-      <c r="K62" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>200</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63" t="s">
+        <v>32</v>
+      </c>
+      <c r="E63" t="s">
+        <v>198</v>
+      </c>
+      <c r="F63" t="s">
+        <v>199</v>
+      </c>
+      <c r="G63" t="s">
+        <v>65</v>
+      </c>
+      <c r="H63" t="s">
+        <v>104</v>
+      </c>
+      <c r="I63" t="s">
+        <v>105</v>
+      </c>
+      <c r="J63" t="s">
+        <v>12</v>
+      </c>
+      <c r="K63" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>201</v>
       </c>
-      <c r="B63">
-        <v>0</v>
-      </c>
-      <c r="C63">
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
         <v>62.02</v>
       </c>
-      <c r="D63">
+      <c r="D64">
         <v>111.489</v>
       </c>
-      <c r="E63">
+      <c r="E64">
         <v>175.54300000000001</v>
       </c>
-      <c r="F63">
+      <c r="F64">
         <v>177.071</v>
       </c>
-      <c r="G63">
+      <c r="G64">
         <v>73.584999999999994</v>
       </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
-      <c r="I63">
-        <v>0</v>
-      </c>
-      <c r="J63">
-        <v>0</v>
-      </c>
-      <c r="K63">
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
         <v>599.70799999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="11">
         <v>38018</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>210</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>84</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>212</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D69" t="s">
         <v>32</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E69" t="s">
         <v>45</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F69" t="s">
         <v>64</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G69" t="s">
         <v>65</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H69" t="s">
         <v>104</v>
       </c>
-      <c r="I68" t="s">
+      <c r="I69" t="s">
         <v>105</v>
       </c>
-      <c r="J68" t="s">
+      <c r="J69" t="s">
         <v>213</v>
       </c>
-      <c r="K68" t="s">
+      <c r="K69" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>16</v>
-      </c>
-      <c r="C69">
-        <v>34</v>
-      </c>
-      <c r="D69">
-        <v>60</v>
-      </c>
-      <c r="E69">
-        <v>97</v>
-      </c>
-      <c r="F69">
-        <v>93</v>
-      </c>
-      <c r="G69">
-        <v>33</v>
-      </c>
-      <c r="K69">
-        <v>317</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>17</v>
-      </c>
-      <c r="B70">
-        <v>3.3</v>
+        <v>16</v>
       </c>
       <c r="C70">
-        <v>63.1</v>
+        <v>34</v>
       </c>
       <c r="D70">
-        <v>106.2</v>
+        <v>60</v>
       </c>
       <c r="E70">
-        <v>175.9</v>
+        <v>97</v>
       </c>
       <c r="F70">
-        <v>184</v>
+        <v>93</v>
       </c>
       <c r="G70">
-        <v>77.400000000000006</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-      <c r="I70">
-        <v>0</v>
-      </c>
-      <c r="J70">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="K70">
-        <v>609.79999999999995</v>
+        <v>317</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="C71">
-        <v>3.7</v>
+        <v>63.1</v>
       </c>
       <c r="D71">
-        <v>6.7</v>
+        <v>106.2</v>
       </c>
       <c r="E71">
-        <v>11.3</v>
+        <v>175.9</v>
       </c>
       <c r="F71">
-        <v>10.8</v>
+        <v>184</v>
       </c>
       <c r="G71">
-        <v>3.8</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -8231,30 +8196,30 @@
         <v>0</v>
       </c>
       <c r="K71">
-        <v>36.4</v>
+        <v>609.79999999999995</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B72">
-        <v>7.7</v>
+        <v>0</v>
       </c>
       <c r="C72">
-        <v>2.8</v>
+        <v>3.7</v>
       </c>
       <c r="D72">
+        <v>6.7</v>
+      </c>
+      <c r="E72">
         <v>11.3</v>
       </c>
-      <c r="E72">
+      <c r="F72">
         <v>10.8</v>
       </c>
-      <c r="F72">
+      <c r="G72">
         <v>3.8</v>
-      </c>
-      <c r="G72">
-        <v>0</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -8271,25 +8236,25 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B73">
-        <v>11</v>
+        <v>7.7</v>
       </c>
       <c r="C73">
-        <v>62.2</v>
+        <v>2.8</v>
       </c>
       <c r="D73">
-        <v>110.7</v>
+        <v>11.3</v>
       </c>
       <c r="E73">
-        <v>175.4</v>
+        <v>10.8</v>
       </c>
       <c r="F73">
-        <v>177</v>
+        <v>3.8</v>
       </c>
       <c r="G73">
-        <v>73.599999999999994</v>
+        <v>0</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -8301,33 +8266,33 @@
         <v>0</v>
       </c>
       <c r="K73">
-        <v>609.79999999999995</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>62.2</v>
       </c>
       <c r="D74">
-        <v>2.2999999999999998</v>
+        <v>110.7</v>
       </c>
       <c r="E74">
-        <v>4.5</v>
+        <v>175.4</v>
       </c>
       <c r="F74">
-        <v>4.5999999999999996</v>
+        <v>177</v>
       </c>
       <c r="G74">
-        <v>1.1000000000000001</v>
+        <v>73.599999999999994</v>
       </c>
       <c r="H74">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="I74">
         <v>0</v>
@@ -8336,30 +8301,30 @@
         <v>0</v>
       </c>
       <c r="K74">
-        <v>13.4</v>
+        <v>609.79999999999995</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B75">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C75">
-        <v>62.2</v>
+        <v>0</v>
       </c>
       <c r="D75">
-        <v>113</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E75">
-        <v>179.9</v>
+        <v>4.5</v>
       </c>
       <c r="F75">
-        <v>181.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="G75">
-        <v>74.599999999999994</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H75">
         <v>0.9</v>
@@ -8371,16 +8336,51 @@
         <v>0</v>
       </c>
       <c r="K75">
-        <v>623.20000000000005</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="B76">
+        <v>11</v>
+      </c>
+      <c r="C76">
+        <v>62.2</v>
+      </c>
+      <c r="D76">
+        <v>113</v>
+      </c>
+      <c r="E76">
+        <v>179.9</v>
+      </c>
+      <c r="F76">
+        <v>181.6</v>
+      </c>
+      <c r="G76">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="H76">
+        <v>0.9</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76">
+        <v>623.20000000000005</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed date match up problem that came from the way we were inputing dates from excel. Also copied over cost variance data for those SARS  taht were missing it.
</commit_message>
<xml_diff>
--- a/FOIA SAR data/LW155 M777/All Docs_M777 Data Draw.xlsx
+++ b/FOIA SAR data/LW155 M777/All Docs_M777 Data Draw.xlsx
@@ -749,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -783,11 +783,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3607,12 +3612,12 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -3857,12 +3862,12 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -4054,12 +4059,12 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
@@ -4275,12 +4280,12 @@
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
@@ -4553,12 +4558,12 @@
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="15" t="s">
+      <c r="A68" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B68" s="15"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
@@ -4771,12 +4776,12 @@
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A82" s="15" t="s">
+      <c r="A82" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B82" s="15"/>
-      <c r="C82" s="15"/>
-      <c r="D82" s="15"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
@@ -5290,12 +5295,12 @@
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A111" s="15" t="s">
+      <c r="A111" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B111" s="15"/>
-      <c r="C111" s="15"/>
-      <c r="D111" s="15"/>
+      <c r="B111" s="14"/>
+      <c r="C111" s="14"/>
+      <c r="D111" s="14"/>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
@@ -5553,12 +5558,12 @@
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A125" s="15" t="s">
+      <c r="A125" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B125" s="15"/>
-      <c r="C125" s="15"/>
-      <c r="D125" s="15"/>
+      <c r="B125" s="14"/>
+      <c r="C125" s="14"/>
+      <c r="D125" s="14"/>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
@@ -5798,12 +5803,12 @@
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A139" s="15" t="s">
+      <c r="A139" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B139" s="15"/>
-      <c r="C139" s="15"/>
-      <c r="D139" s="15"/>
+      <c r="B139" s="14"/>
+      <c r="C139" s="14"/>
+      <c r="D139" s="14"/>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
@@ -5971,12 +5976,12 @@
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A153" s="15" t="s">
+      <c r="A153" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B153" s="15"/>
-      <c r="C153" s="15"/>
-      <c r="D153" s="15"/>
+      <c r="B153" s="14"/>
+      <c r="C153" s="14"/>
+      <c r="D153" s="14"/>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
@@ -6126,12 +6131,12 @@
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A167" s="15" t="s">
+      <c r="A167" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B167" s="15"/>
-      <c r="C167" s="15"/>
-      <c r="D167" s="15"/>
+      <c r="B167" s="14"/>
+      <c r="C167" s="14"/>
+      <c r="D167" s="14"/>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
@@ -6314,12 +6319,12 @@
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A181" s="14" t="s">
+      <c r="A181" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B181" s="14"/>
-      <c r="C181" s="14"/>
-      <c r="D181" s="14"/>
+      <c r="B181" s="15"/>
+      <c r="C181" s="15"/>
+      <c r="D181" s="15"/>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
@@ -6616,12 +6621,12 @@
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A192" s="14" t="s">
+      <c r="A192" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B192" s="14"/>
-      <c r="C192" s="14"/>
-      <c r="D192" s="14"/>
+      <c r="B192" s="15"/>
+      <c r="C192" s="15"/>
+      <c r="D192" s="15"/>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
@@ -6909,11 +6914,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A192:D192"/>
+    <mergeCell ref="A111:D111"/>
+    <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A139:D139"/>
+    <mergeCell ref="A153:D153"/>
+    <mergeCell ref="A167:D167"/>
+    <mergeCell ref="A181:D181"/>
     <mergeCell ref="B94:D94"/>
     <mergeCell ref="E94:G94"/>
     <mergeCell ref="H94:J94"/>
@@ -6922,13 +6929,11 @@
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A68:D68"/>
     <mergeCell ref="A82:D82"/>
-    <mergeCell ref="A192:D192"/>
-    <mergeCell ref="A111:D111"/>
-    <mergeCell ref="A125:D125"/>
-    <mergeCell ref="A139:D139"/>
-    <mergeCell ref="A153:D153"/>
-    <mergeCell ref="A167:D167"/>
-    <mergeCell ref="A181:D181"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6939,13 +6944,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.28515625" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
@@ -6956,12 +6961,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="11">
+      <c r="A1" s="16">
         <v>35462</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="17" t="s">
         <v>192</v>
       </c>
       <c r="B2" t="s">
@@ -6969,7 +6974,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="18" t="s">
         <v>193</v>
       </c>
       <c r="B3" t="s">
@@ -6977,7 +6982,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="18" t="s">
         <v>196</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -7012,7 +7017,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="18" t="s">
         <v>220</v>
       </c>
       <c r="B5">
@@ -7047,12 +7052,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="18" t="s">
         <v>200</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -7087,7 +7092,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="18" t="s">
         <v>201</v>
       </c>
       <c r="B8">
@@ -7122,12 +7127,12 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="A10" s="16">
         <v>35827</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="17" t="s">
         <v>192</v>
       </c>
       <c r="B11" t="s">
@@ -7135,7 +7140,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="18" t="s">
         <v>193</v>
       </c>
       <c r="B12" t="s">
@@ -7143,7 +7148,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="18" t="s">
         <v>196</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -7175,7 +7180,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="18" t="s">
         <v>203</v>
       </c>
       <c r="B14">
@@ -7207,12 +7212,12 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="18" t="s">
         <v>200</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -7245,7 +7250,7 @@
       <c r="K16" s="12"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="18" t="s">
         <v>201</v>
       </c>
       <c r="B17">
@@ -7277,12 +7282,12 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
+      <c r="A19" s="16">
         <v>36192</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="17" t="s">
         <v>192</v>
       </c>
       <c r="B20" t="s">
@@ -7290,7 +7295,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="18" t="s">
         <v>214</v>
       </c>
       <c r="B21" t="s">
@@ -7298,7 +7303,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="18" t="s">
         <v>196</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -7333,7 +7338,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="18" t="s">
         <v>218</v>
       </c>
       <c r="B23">
@@ -7368,12 +7373,12 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="18" t="s">
         <v>200</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -7408,7 +7413,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="18" t="s">
         <v>201</v>
       </c>
       <c r="B26">
@@ -7443,12 +7448,12 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
+      <c r="A28" s="16">
         <v>36557</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="17" t="s">
         <v>192</v>
       </c>
       <c r="B29" t="s">
@@ -7456,7 +7461,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="18" t="s">
         <v>193</v>
       </c>
       <c r="B30" t="s">
@@ -7464,7 +7469,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="18" t="s">
         <v>196</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -7496,7 +7501,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="18" t="s">
         <v>203</v>
       </c>
       <c r="B32">
@@ -7528,12 +7533,12 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="18" t="s">
         <v>200</v>
       </c>
       <c r="B35" s="12" t="s">
@@ -7568,7 +7573,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="18" t="s">
         <v>201</v>
       </c>
       <c r="B36">
@@ -7603,12 +7608,12 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+      <c r="A38" s="16">
         <v>37043</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="17" t="s">
         <v>192</v>
       </c>
       <c r="B39" t="s">
@@ -7616,7 +7621,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="18" t="s">
         <v>193</v>
       </c>
       <c r="B40" t="s">
@@ -7624,7 +7629,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="18" t="s">
         <v>196</v>
       </c>
       <c r="B41" t="s">
@@ -7659,7 +7664,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="18" t="s">
         <v>197</v>
       </c>
       <c r="B42">
@@ -7694,12 +7699,12 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="18" t="s">
         <v>200</v>
       </c>
       <c r="B44" t="s">
@@ -7734,7 +7739,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="18" t="s">
         <v>201</v>
       </c>
       <c r="B45">
@@ -7769,12 +7774,12 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
+      <c r="A47" s="16">
         <v>37288</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="17" t="s">
         <v>192</v>
       </c>
       <c r="B48" t="s">
@@ -7782,7 +7787,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="18" t="s">
         <v>193</v>
       </c>
       <c r="B49" t="s">
@@ -7790,7 +7795,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="18" t="s">
         <v>196</v>
       </c>
       <c r="B50" s="4" t="s">
@@ -7822,7 +7827,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="18" t="s">
         <v>197</v>
       </c>
       <c r="B51">
@@ -7854,12 +7859,12 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="18" t="s">
         <v>200</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -7891,7 +7896,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="18" t="s">
         <v>201</v>
       </c>
       <c r="B54">
@@ -7923,12 +7928,12 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="11">
+      <c r="A57" s="16">
         <v>37653</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="17" t="s">
         <v>192</v>
       </c>
       <c r="B58" t="s">
@@ -7936,7 +7941,7 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="18" t="s">
         <v>193</v>
       </c>
       <c r="B59" t="s">
@@ -7944,7 +7949,7 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="18" t="s">
         <v>196</v>
       </c>
       <c r="B60" s="4" t="s">
@@ -7979,7 +7984,7 @@
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" s="18" t="s">
         <v>197</v>
       </c>
       <c r="B61">
@@ -8014,12 +8019,12 @@
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="18" t="s">
         <v>200</v>
       </c>
       <c r="B63" s="4" t="s">
@@ -8054,7 +8059,7 @@
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="18" t="s">
         <v>201</v>
       </c>
       <c r="B64">
@@ -8089,12 +8094,12 @@
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="11">
+      <c r="A66" s="16">
         <v>38018</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="17" t="s">
         <v>192</v>
       </c>
       <c r="B67" t="s">
@@ -8102,7 +8107,7 @@
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="18" t="s">
         <v>210</v>
       </c>
       <c r="B68" t="s">
@@ -8142,7 +8147,7 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="18" t="s">
         <v>16</v>
       </c>
       <c r="C70">
@@ -8165,7 +8170,7 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B71">
@@ -8200,7 +8205,7 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="18" t="s">
         <v>18</v>
       </c>
       <c r="B72">
@@ -8235,7 +8240,7 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="A73" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B73">
@@ -8270,7 +8275,7 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="18" t="s">
         <v>20</v>
       </c>
       <c r="B74">
@@ -8305,7 +8310,7 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="A75" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B75">
@@ -8340,7 +8345,7 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="A76" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B76">
@@ -8375,12 +8380,12 @@
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="A77" s="18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="A78" s="18" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>